<commit_message>
add data into excel file
</commit_message>
<xml_diff>
--- a/database/data_gv.xlsx
+++ b/database/data_gv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DangKyHocPhan\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCDC82B-609F-479E-B161-8A833E1479D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C881DC-06A3-4736-A68E-3F42CA01201C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9684" xr2:uid="{9D347ADD-5C74-43DD-A1DF-D52A9FCA7969}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>magv</t>
   </si>
@@ -88,6 +88,66 @@
   </si>
   <si>
     <t>KCB</t>
+  </si>
+  <si>
+    <t>GV005</t>
+  </si>
+  <si>
+    <t>Đặng Thế Hiếu</t>
+  </si>
+  <si>
+    <t>dangthehieu@gmail.com</t>
+  </si>
+  <si>
+    <t>GV006</t>
+  </si>
+  <si>
+    <t>Võ Văn Tuấn</t>
+  </si>
+  <si>
+    <t>tuanvo@gmail.com</t>
+  </si>
+  <si>
+    <t>GV007</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn Anh</t>
+  </si>
+  <si>
+    <t>tuananh@gmail.com</t>
+  </si>
+  <si>
+    <t>KCS</t>
+  </si>
+  <si>
+    <t>GV008</t>
+  </si>
+  <si>
+    <t>Nguyễn Kim Chi</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>kimchi@gmail.com</t>
+  </si>
+  <si>
+    <t>GV009</t>
+  </si>
+  <si>
+    <t>Bùi Công Nam</t>
+  </si>
+  <si>
+    <t>congnam@gmail.com</t>
+  </si>
+  <si>
+    <t>GV010</t>
+  </si>
+  <si>
+    <t>Lê Thị Giang</t>
+  </si>
+  <si>
+    <t>legiang@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -449,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9DA6DF-116B-42EE-8CCC-D8E954929616}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -550,6 +610,108 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>